<commit_message>
fipy conversion to zeta
</commit_message>
<xml_diff>
--- a/output/compu_times.xlsx
+++ b/output/compu_times.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\blopti_dev\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAA562F-B843-46F4-A313-C3FA7969302C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD2816E-ACE2-4DF9-BE46-2F9475B76F56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="21270" xr2:uid="{D0F69822-F806-4922-84DB-E01FA1D1B213}"/>
+    <workbookView xWindow="2415" yWindow="2580" windowWidth="26055" windowHeight="13470" activeTab="1" xr2:uid="{D0F69822-F806-4922-84DB-E01FA1D1B213}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="solution_methods" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>ncpu</t>
   </si>
@@ -75,6 +76,42 @@
   </si>
   <si>
     <t>Too"straight up" S and T? Hmm…</t>
+  </si>
+  <si>
+    <t>15-Oct</t>
+  </si>
+  <si>
+    <t>Jacobian with loops</t>
+  </si>
+  <si>
+    <t>Jacobian vectorial</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>tolerance residue</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>FiPy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J and F vectorial </t>
+  </si>
+  <si>
+    <t>solver</t>
+  </si>
+  <si>
+    <t>np.linalg.solve</t>
+  </si>
+  <si>
+    <t>J banded and F vectorial</t>
+  </si>
+  <si>
+    <t>scipy.solve.banded with all options for performance</t>
   </si>
 </sst>
 </file>
@@ -118,13 +155,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A053CB1-4BDA-462A-9AB3-F85BF27A04FC}">
-  <dimension ref="A2:I4"/>
+  <dimension ref="A2:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,6 +577,122 @@
         <v>13</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C2B4891-6638-4DEA-9BF8-58C84DFDAE1A}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>